<commit_message>
confirmed NZIP and FOIA similar outcomes
</commit_message>
<xml_diff>
--- a/data/FOIA/KCOR_summary.xlsx
+++ b/data/FOIA/KCOR_summary.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.5140</t>
+          <t>1.3371</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.470</t>
+          <t>1.298</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.559</t>
+          <t>1.377</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.1672</t>
+          <t>1.1771</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.077</t>
+          <t>1.085</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.265</t>
+          <t>1.277</t>
         </is>
       </c>
     </row>
@@ -540,17 +540,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.2232</t>
+          <t>1.0932</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.177</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.272</t>
+          <t>1.137</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.7971</t>
+          <t>1.5055</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.734</t>
+          <t>1.452</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.862</t>
+          <t>1.561</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.6427</t>
+          <t>1.4943</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.509</t>
+          <t>1.372</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.788</t>
+          <t>1.627</t>
         </is>
       </c>
     </row>
@@ -609,17 +609,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.7049</t>
+          <t>1.1500</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.422</t>
+          <t>0.957</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2.044</t>
+          <t>1.381</t>
         </is>
       </c>
     </row>
@@ -632,17 +632,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.7548</t>
+          <t>1.5595</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.306</t>
+          <t>1.160</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.357</t>
+          <t>2.097</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.9137</t>
+          <t>3.7045</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>2.002</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3.573</t>
+          <t>6.855</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.5243</t>
+          <t>1.0637</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>15.243</t>
+          <t>10.637</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.3085</t>
+          <t>11.9874</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>73.085</t>
+          <t>119.874</t>
         </is>
       </c>
     </row>
@@ -742,17 +742,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.6989</t>
+          <t>1.7833</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.642</t>
+          <t>1.724</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.758</t>
+          <t>1.845</t>
         </is>
       </c>
     </row>
@@ -765,17 +765,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.5377</t>
+          <t>1.7067</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.444</t>
+          <t>1.602</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.637</t>
+          <t>1.819</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.9166</t>
+          <t>1.8895</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.848</t>
+          <t>1.822</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.987</t>
+          <t>1.960</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.7802</t>
+          <t>1.4692</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.684</t>
+          <t>1.389</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.882</t>
+          <t>1.554</t>
         </is>
       </c>
     </row>
@@ -834,17 +834,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.4772</t>
+          <t>1.3436</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>1.209</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.640</t>
+          <t>1.494</t>
         </is>
       </c>
     </row>
@@ -857,17 +857,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.6011</t>
+          <t>9.3548</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.313</t>
+          <t>7.712</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.952</t>
+          <t>11.347</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.5393</t>
+          <t>1.6700</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>1.195</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2.150</t>
+          <t>2.333</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.7654</t>
+          <t>1.5687</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.514</t>
+          <t>1.056</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>2.329</t>
         </is>
       </c>
     </row>
@@ -926,17 +926,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2.1472</t>
+          <t>5.9260</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>2.488</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>5.200</t>
+          <t>14.115</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.8932</t>
+          <t>4.7454</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>28.932</t>
+          <t>47.454</t>
         </is>
       </c>
     </row>
@@ -990,17 +990,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1202</t>
+          <t>1.3213</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.073</t>
+          <t>1.266</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>1.379</t>
         </is>
       </c>
     </row>
@@ -1013,17 +1013,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.3174</t>
+          <t>1.4499</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>1.326</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.439</t>
+          <t>1.585</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.5668</t>
+          <t>1.7283</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.496</t>
+          <t>1.650</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.641</t>
+          <t>1.810</t>
         </is>
       </c>
     </row>
@@ -1059,17 +1059,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.9906</t>
+          <t>0.9759</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.930</t>
+          <t>0.916</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.039</t>
         </is>
       </c>
     </row>
@@ -1082,17 +1082,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.8993</t>
+          <t>0.8991</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.788</t>
+          <t>0.786</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.028</t>
         </is>
       </c>
     </row>
@@ -1105,17 +1105,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9391</t>
+          <t>8.1350</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.720</t>
+          <t>6.251</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.225</t>
+          <t>10.586</t>
         </is>
       </c>
     </row>
@@ -1128,17 +1128,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.8772</t>
+          <t>1.0709</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.564</t>
+          <t>0.688</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.365</t>
+          <t>1.668</t>
         </is>
       </c>
     </row>
@@ -1151,17 +1151,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.4000</t>
+          <t>0.4235</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.192</t>
+          <t>0.205</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.874</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.1019</t>
+          <t>4.5859</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>11.019</t>
+          <t>45.859</t>
         </is>
       </c>
     </row>
@@ -1295,17 +1295,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2073</t>
+          <t>1.0869</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.173</t>
+          <t>1.056</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.242</t>
+          <t>1.119</t>
         </is>
       </c>
     </row>
@@ -1318,17 +1318,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9856</t>
+          <t>1.0653</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.891</t>
+          <t>0.962</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.090</t>
+          <t>1.180</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0622</t>
+          <t>1.0086</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>0.954</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.122</t>
+          <t>1.066</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2512</t>
+          <t>1.0008</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.195</t>
+          <t>0.955</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.310</t>
+          <t>1.048</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.4154</t>
+          <t>1.2514</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.342</t>
+          <t>1.186</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.493</t>
+          <t>1.320</t>
         </is>
       </c>
     </row>
@@ -1410,17 +1410,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.3753</t>
+          <t>1.3333</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.270</t>
+          <t>1.231</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.490</t>
+          <t>1.445</t>
         </is>
       </c>
     </row>
@@ -1433,17 +1433,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.3035</t>
+          <t>1.2669</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.159</t>
+          <t>1.126</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.466</t>
+          <t>1.426</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0022</t>
+          <t>0.6432</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.806</t>
+          <t>0.515</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.247</t>
+          <t>0.803</t>
         </is>
       </c>
     </row>
@@ -1479,17 +1479,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4.9169</t>
+          <t>2.5037</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2.026</t>
+          <t>0.989</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>11.932</t>
+          <t>6.337</t>
         </is>
       </c>
     </row>
@@ -1502,17 +1502,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.2852</t>
+          <t>2.4289</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.524</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3.153</t>
+          <t>5.922</t>
         </is>
       </c>
     </row>
@@ -1543,17 +1543,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.3727</t>
+          <t>1.2232</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.342</t>
+          <t>1.195</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.405</t>
+          <t>1.252</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1210</t>
+          <t>1.1802</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.191</t>
+          <t>1.255</t>
         </is>
       </c>
     </row>
@@ -1589,17 +1589,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.2042</t>
+          <t>1.0805</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.162</t>
+          <t>1.043</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.247</t>
+          <t>1.120</t>
         </is>
       </c>
     </row>
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.4592</t>
+          <t>1.1329</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.408</t>
+          <t>1.093</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.512</t>
+          <t>1.174</t>
         </is>
       </c>
     </row>
@@ -1635,17 +1635,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.6855</t>
+          <t>1.4980</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.597</t>
+          <t>1.419</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.779</t>
+          <t>1.581</t>
         </is>
       </c>
     </row>
@@ -1658,17 +1658,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.4263</t>
+          <t>1.5967</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.290</t>
+          <t>1.444</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.577</t>
+          <t>1.766</t>
         </is>
       </c>
     </row>
@@ -1681,17 +1681,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.4654</t>
+          <t>1.8078</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.244</t>
+          <t>1.535</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.727</t>
+          <t>2.129</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.3639</t>
+          <t>3.6752</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>2.733</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.849</t>
+          <t>4.943</t>
         </is>
       </c>
     </row>
@@ -1727,17 +1727,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.3154</t>
+          <t>1.6161</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.832</t>
+          <t>1.022</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2.079</t>
+          <t>2.555</t>
         </is>
       </c>
     </row>
@@ -1750,17 +1750,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.3893</t>
+          <t>0.4741</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.566</t>
+          <t>0.178</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3.408</t>
+          <t>1.263</t>
         </is>
       </c>
     </row>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1370</t>
+          <t>1.1254</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>1.090</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.173</t>
+          <t>1.162</t>
         </is>
       </c>
     </row>
@@ -1814,17 +1814,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.1375</t>
+          <t>1.1079</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.031</t>
+          <t>1.003</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.255</t>
+          <t>1.223</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.1337</t>
+          <t>1.0713</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.075</t>
+          <t>1.016</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.195</t>
+          <t>1.130</t>
         </is>
       </c>
     </row>
@@ -1860,17 +1860,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1663</t>
+          <t>1.1320</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.113</t>
+          <t>1.080</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.222</t>
+          <t>1.187</t>
         </is>
       </c>
     </row>
@@ -1883,17 +1883,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.1908</t>
+          <t>1.1971</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.122</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.270</t>
+          <t>1.278</t>
         </is>
       </c>
     </row>
@@ -1906,17 +1906,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0371</t>
+          <t>1.1976</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.923</t>
+          <t>1.066</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.165</t>
+          <t>1.346</t>
         </is>
       </c>
     </row>
@@ -1929,17 +1929,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.1242</t>
+          <t>1.4269</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.932</t>
+          <t>1.183</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.356</t>
+          <t>1.721</t>
         </is>
       </c>
     </row>
@@ -1952,17 +1952,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.3610</t>
+          <t>5.7141</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.954</t>
+          <t>4.026</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.941</t>
+          <t>8.109</t>
         </is>
       </c>
     </row>
@@ -1975,17 +1975,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.2675</t>
+          <t>0.6455</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.100</t>
+          <t>0.233</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.713</t>
+          <t>1.788</t>
         </is>
       </c>
     </row>
@@ -1998,17 +1998,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.0810</t>
+          <t>0.1952</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.312</t>
+          <t>0.053</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>3.739</t>
+          <t>0.714</t>
         </is>
       </c>
     </row>
@@ -2096,17 +2096,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0327</t>
+          <t>1.0796</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.989</t>
+          <t>1.033</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>1.128</t>
         </is>
       </c>
     </row>
@@ -2119,17 +2119,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.2003</t>
+          <t>1.1459</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>0.937</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.465</t>
+          <t>1.402</t>
         </is>
       </c>
     </row>
@@ -2142,17 +2142,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0979</t>
+          <t>1.1027</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.008</t>
+          <t>1.012</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.196</t>
+          <t>1.202</t>
         </is>
       </c>
     </row>
@@ -2165,17 +2165,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9312</t>
+          <t>0.9529</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.866</t>
+          <t>0.886</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.002</t>
+          <t>1.025</t>
         </is>
       </c>
     </row>
@@ -2188,17 +2188,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1392</t>
+          <t>1.2758</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>1.161</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.252</t>
+          <t>1.402</t>
         </is>
       </c>
     </row>
@@ -2211,17 +2211,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9672</t>
+          <t>1.3862</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.852</t>
+          <t>1.223</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.098</t>
+          <t>1.572</t>
         </is>
       </c>
     </row>
@@ -2234,17 +2234,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9074</t>
+          <t>0.6630</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.770</t>
+          <t>0.562</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>0.783</t>
         </is>
       </c>
     </row>
@@ -2257,17 +2257,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0310</t>
+          <t>1.5807</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.785</t>
+          <t>1.209</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.354</t>
+          <t>2.067</t>
         </is>
       </c>
     </row>
@@ -2280,17 +2280,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.2813</t>
+          <t>1.8362</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.839</t>
+          <t>1.207</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.955</t>
+          <t>2.793</t>
         </is>
       </c>
     </row>
@@ -2303,17 +2303,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.4635</t>
+          <t>2.7393</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.592</t>
+          <t>1.136</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3.620</t>
+          <t>6.603</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0366</t>
+          <t>1.0729</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.014</t>
+          <t>1.049</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>1.097</t>
         </is>
       </c>
     </row>
@@ -2367,17 +2367,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8798</t>
+          <t>0.9211</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.814</t>
+          <t>0.851</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.951</t>
+          <t>0.997</t>
         </is>
       </c>
     </row>
@@ -2390,17 +2390,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0624</t>
+          <t>1.0926</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.020</t>
+          <t>1.049</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.107</t>
+          <t>1.139</t>
         </is>
       </c>
     </row>
@@ -2413,17 +2413,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9894</t>
+          <t>0.9800</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.952</t>
+          <t>0.943</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>1.019</t>
         </is>
       </c>
     </row>
@@ -2436,17 +2436,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1128</t>
+          <t>1.2366</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.059</t>
+          <t>1.176</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.170</t>
+          <t>1.300</t>
         </is>
       </c>
     </row>
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0641</t>
+          <t>1.3690</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>1.269</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.148</t>
+          <t>1.477</t>
         </is>
       </c>
     </row>
@@ -2482,17 +2482,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.2126</t>
+          <t>1.0223</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.089</t>
+          <t>0.918</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.350</t>
+          <t>1.139</t>
         </is>
       </c>
     </row>
@@ -2505,17 +2505,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2266</t>
+          <t>1.2667</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.056</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.473</t>
+          <t>1.520</t>
         </is>
       </c>
     </row>
@@ -2528,17 +2528,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.4245</t>
+          <t>1.4463</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.076</t>
+          <t>1.091</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.887</t>
+          <t>1.917</t>
         </is>
       </c>
     </row>
@@ -2551,17 +2551,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.4917</t>
+          <t>1.1467</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.023</t>
+          <t>0.782</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.176</t>
+          <t>1.681</t>
         </is>
       </c>
     </row>
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.0037</t>
+          <t>0.9938</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>0.951</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.049</t>
+          <t>1.039</t>
         </is>
       </c>
     </row>
@@ -2615,17 +2615,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.7329</t>
+          <t>0.8038</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.599</t>
+          <t>0.655</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.896</t>
+          <t>0.986</t>
         </is>
       </c>
     </row>
@@ -2638,17 +2638,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9677</t>
+          <t>0.9909</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>0.908</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.081</t>
         </is>
       </c>
     </row>
@@ -2661,17 +2661,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0625</t>
+          <t>1.0284</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.988</t>
+          <t>0.956</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.143</t>
+          <t>1.107</t>
         </is>
       </c>
     </row>
@@ -2684,17 +2684,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.9768</t>
+          <t>0.9693</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>0.880</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.076</t>
+          <t>1.068</t>
         </is>
       </c>
     </row>
@@ -2707,17 +2707,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.1002</t>
+          <t>0.9876</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.866</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.256</t>
+          <t>1.126</t>
         </is>
       </c>
     </row>
@@ -2730,17 +2730,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.3363</t>
+          <t>1.5418</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.122</t>
+          <t>1.292</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.591</t>
+          <t>1.840</t>
         </is>
       </c>
     </row>
@@ -2753,17 +2753,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.1897</t>
+          <t>0.8014</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.597</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.603</t>
+          <t>1.076</t>
         </is>
       </c>
     </row>
@@ -2776,17 +2776,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.1118</t>
+          <t>0.7876</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.703</t>
+          <t>0.499</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.759</t>
+          <t>1.242</t>
         </is>
       </c>
     </row>
@@ -2799,17 +2799,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.0192</t>
+          <t>0.4186</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.401</t>
+          <t>0.169</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2.592</t>
+          <t>1.040</t>
         </is>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.6273</t>
+          <t>1.4572</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.596</t>
+          <t>1.429</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.659</t>
+          <t>1.486</t>
         </is>
       </c>
     </row>
@@ -2863,17 +2863,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.2587</t>
+          <t>1.2948</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.180</t>
+          <t>1.213</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.342</t>
+          <t>1.382</t>
         </is>
       </c>
     </row>
@@ -2886,17 +2886,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.6019</t>
+          <t>1.4760</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.548</t>
+          <t>1.426</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.658</t>
+          <t>1.528</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.7443</t>
+          <t>1.5188</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.686</t>
+          <t>1.467</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.805</t>
+          <t>1.572</t>
         </is>
       </c>
     </row>
@@ -2932,17 +2932,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.7016</t>
+          <t>1.4994</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.627</t>
+          <t>1.433</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.780</t>
+          <t>1.569</t>
         </is>
       </c>
     </row>
@@ -2955,17 +2955,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.3801</t>
+          <t>1.3274</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.282</t>
+          <t>1.232</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.486</t>
+          <t>1.430</t>
         </is>
       </c>
     </row>
@@ -2978,17 +2978,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.6585</t>
+          <t>1.3160</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.470</t>
+          <t>1.166</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.871</t>
+          <t>1.485</t>
         </is>
       </c>
     </row>
@@ -3001,17 +3001,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.2032</t>
+          <t>0.6186</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.987</t>
+          <t>0.505</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.466</t>
+          <t>0.758</t>
         </is>
       </c>
     </row>
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.6230</t>
+          <t>0.9699</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.125</t>
+          <t>0.665</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2.341</t>
+          <t>1.414</t>
         </is>
       </c>
     </row>
@@ -3047,17 +3047,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.1634</t>
+          <t>1.5711</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.670</t>
+          <t>0.907</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2.020</t>
+          <t>2.721</t>
         </is>
       </c>
     </row>
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5757</t>
+          <t>1.3498</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.510</t>
+          <t>1.293</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.645</t>
+          <t>1.409</t>
         </is>
       </c>
     </row>
@@ -3111,17 +3111,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.0486</t>
+          <t>1.1299</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.862</t>
+          <t>0.926</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.276</t>
+          <t>1.379</t>
         </is>
       </c>
     </row>
@@ -3134,17 +3134,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.4591</t>
+          <t>1.3385</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.342</t>
+          <t>1.230</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.587</t>
+          <t>1.456</t>
         </is>
       </c>
     </row>
@@ -3157,17 +3157,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.8730</t>
+          <t>1.5939</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.745</t>
+          <t>1.484</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2.011</t>
+          <t>1.711</t>
         </is>
       </c>
     </row>
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.4936</t>
+          <t>1.1753</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.359</t>
+          <t>1.069</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.642</t>
+          <t>1.292</t>
         </is>
       </c>
     </row>
@@ -3203,17 +3203,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.4269</t>
+          <t>0.9576</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.251</t>
+          <t>0.841</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.627</t>
+          <t>1.091</t>
         </is>
       </c>
     </row>
@@ -3226,17 +3226,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.8277</t>
+          <t>1.9848</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.522</t>
+          <t>1.649</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2.194</t>
+          <t>2.389</t>
         </is>
       </c>
     </row>
@@ -3249,17 +3249,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.1670</t>
+          <t>0.3914</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.858</t>
+          <t>0.288</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.587</t>
+          <t>0.533</t>
         </is>
       </c>
     </row>
@@ -3272,17 +3272,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.2668</t>
+          <t>0.5282</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.756</t>
+          <t>0.314</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2.121</t>
+          <t>0.888</t>
         </is>
       </c>
     </row>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.7949</t>
+          <t>0.5736</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.288</t>
+          <t>0.213</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2.197</t>
+          <t>1.546</t>
         </is>
       </c>
     </row>
@@ -3336,17 +3336,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.5698</t>
+          <t>1.3582</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>1.330</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.602</t>
+          <t>1.387</t>
         </is>
       </c>
     </row>
@@ -3359,17 +3359,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1.4307</t>
+          <t>1.4057</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.308</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.536</t>
+          <t>1.510</t>
         </is>
       </c>
     </row>
@@ -3382,17 +3382,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.5078</t>
+          <t>1.3509</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.453</t>
+          <t>1.302</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.564</t>
+          <t>1.402</t>
         </is>
       </c>
     </row>
@@ -3405,17 +3405,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.7629</t>
+          <t>1.5498</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.703</t>
+          <t>1.496</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.825</t>
+          <t>1.605</t>
         </is>
       </c>
     </row>
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1.5290</t>
+          <t>1.2125</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.455</t>
+          <t>1.153</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1.607</t>
+          <t>1.275</t>
         </is>
       </c>
     </row>
@@ -3451,17 +3451,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.2970</t>
+          <t>0.9696</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.193</t>
+          <t>0.892</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.409</t>
+          <t>1.054</t>
         </is>
       </c>
     </row>
@@ -3474,17 +3474,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.3677</t>
+          <t>1.2873</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.196</t>
+          <t>1.125</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.564</t>
+          <t>1.474</t>
         </is>
       </c>
     </row>
@@ -3497,17 +3497,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0.9809</t>
+          <t>0.4884</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.777</t>
+          <t>0.385</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.238</t>
+          <t>0.619</t>
         </is>
       </c>
     </row>
@@ -3520,17 +3520,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.1394</t>
+          <t>0.6706</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.758</t>
+          <t>0.442</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.712</t>
+          <t>1.018</t>
         </is>
       </c>
     </row>
@@ -3543,17 +3543,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>0.7799</t>
+          <t>1.3701</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.430</t>
+          <t>0.755</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.416</t>
+          <t>2.486</t>
         </is>
       </c>
     </row>

</xml_diff>